<commit_message>
What I think is the final version
</commit_message>
<xml_diff>
--- a/Rebuild-analysis-model.xlsx
+++ b/Rebuild-analysis-model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danjamk/yukon/app-rewrite-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B278E97-ED80-3E46-8E12-6B12C1827F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3F8B99-3015-FC46-B11C-5B58804E00AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41380" yWindow="2080" windowWidth="31320" windowHeight="18320" activeTab="1" xr2:uid="{B5141DE5-0234-B641-953B-82ABCA3098E8}"/>
   </bookViews>
@@ -34,6 +34,24 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={6E664929-2246-064C-A1FF-73FC1D48D61D}</author>
+  </authors>
+  <commentList>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{6E664929-2246-064C-A1FF-73FC1D48D61D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This could be new stack, cloud and now the impact of AI tools.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -108,7 +126,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -135,6 +153,12 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2962,6 +2986,12 @@
 </c:userShapes>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Dan Kuhn" id="{5CA9343B-F00A-D541-ADF9-C0A2D9695DC3}" userId="c24148852a3b88bf" providerId="Windows Live"/>
+</personList>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFF3C0DE-459F-DB48-AD3D-46543C5D0365}" name="Table1" displayName="Table1" ref="A6:D16" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A6:D16" xr:uid="{DFF3C0DE-459F-DB48-AD3D-46543C5D0365}"/>
@@ -3310,6 +3340,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B7" dT="2025-06-10T17:48:55.31" personId="{5CA9343B-F00A-D541-ADF9-C0A2D9695DC3}" id="{6E664929-2246-064C-A1FF-73FC1D48D61D}">
+    <text>This could be new stack, cloud and now the impact of AI tools.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC4CC3E-EF6D-C847-8137-E04C6508D253}">
   <dimension ref="A2:F18"/>
@@ -3565,11 +3603,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8B5A5E-4D62-C74F-BC35-85FE85ABE26C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8B5A5E-4D62-C74F-BC35-85FE85ABE26C}">
   <dimension ref="A3:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S36" sqref="S36"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3841,8 +3879,9 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>